<commit_message>
The excel has been changed, a couple "Discoveries" have been added
</commit_message>
<xml_diff>
--- a/Actividad 01 - Identificación Hallazgos BD.xlsx
+++ b/Actividad 01 - Identificación Hallazgos BD.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keyvin Rosales\Desktop\Activdad01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pamel\Documents\Universidad\CuatrimestreI2025\Auditoría de Sistemas\Auditoria-ISW1012-Actividades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6AE564E-6C16-414C-AAB3-EFF612723324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4BC9E23-2C20-47ED-8934-72C9DB620A43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{124CE4B9-C2B7-444E-982F-07D767DED2D4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{124CE4B9-C2B7-444E-982F-07D767DED2D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Instrucciones" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="67">
   <si>
     <t>#</t>
   </si>
@@ -59,12 +59,6 @@
   </si>
   <si>
     <t>Evaluación</t>
-  </si>
-  <si>
-    <t>Hallazgo 04</t>
-  </si>
-  <si>
-    <t>Hallazgo 05</t>
   </si>
   <si>
     <t>Debilidad</t>
@@ -227,28 +221,31 @@
     <t>En la base de datos ISW1012,en el esquema actividad01, en la tabla producto, existe al menos un registro con el campo nombre vacío (' ').</t>
   </si>
   <si>
-    <t>Columna1</t>
-  </si>
-  <si>
-    <t>Suma</t>
-  </si>
-  <si>
-    <t>Promedio</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Recuento</t>
-  </si>
-  <si>
-    <t>Hallazgo 01-Falta de Restricción de Unicidad en Código de Producto.</t>
-  </si>
-  <si>
-    <t>Hallazgo 02-Productos sin Nombre.</t>
-  </si>
-  <si>
-    <t>Hallazgo 03-Pedidos con Monto Total en Cero.</t>
+    <t>Hallazgo 06</t>
+  </si>
+  <si>
+    <t>Hallazgo 04 - Llave Foránea no Detectada en Detalle de Pedidos hacia Productos.</t>
+  </si>
+  <si>
+    <t>Hallazgo 03 - Pedidos con Monto Total en Cero.</t>
+  </si>
+  <si>
+    <t>Hallazgo 02 - Productos sin Nombre.</t>
+  </si>
+  <si>
+    <t>Hallazgo 01 - Falta de Restricción de Unicidad en Código de Producto.</t>
+  </si>
+  <si>
+    <t>Regla de Integridad Referencial</t>
+  </si>
+  <si>
+    <t>Hallazgo 05 - Fechas Inconsistentes de Creación</t>
+  </si>
+  <si>
+    <t>Regla de Integridad de Negocio</t>
+  </si>
+  <si>
+    <t>Regla de Identidad de Usuario o Dominio</t>
   </si>
 </sst>
 </file>
@@ -475,39 +472,6 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -595,13 +559,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <top style="hair">
           <color auto="1"/>
         </top>
@@ -609,6 +566,46 @@
           <color auto="1"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -628,27 +625,23 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F037A2D3-40B3-416E-AF78-E48342CCEF11}" name="Tabla1" displayName="Tabla1" ref="A1:D19" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="6" tableBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F037A2D3-40B3-416E-AF78-E48342CCEF11}" name="Tabla1" displayName="Tabla1" ref="A1:D19" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4">
   <autoFilter ref="A1:D19" xr:uid="{F037A2D3-40B3-416E-AF78-E48342CCEF11}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{3463565E-DD8D-4BA6-8CF0-1F90763F07F3}" name="#" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{D2E08A89-2CED-4578-9670-D70E2738C313}" name="Debilidad" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{B37DC959-5964-4E10-AA52-EC2194040721}" name="Regla de Integridad" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{87B5B8CE-8756-4E34-8265-06951CB9CC45}" name="Hallazgo" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{3463565E-DD8D-4BA6-8CF0-1F90763F07F3}" name="#" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{D2E08A89-2CED-4578-9670-D70E2738C313}" name="Debilidad" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{B37DC959-5964-4E10-AA52-EC2194040721}" name="Regla de Integridad" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{87B5B8CE-8756-4E34-8265-06951CB9CC45}" name="Hallazgo" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -686,7 +679,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -792,7 +785,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -934,7 +927,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -944,11 +937,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1446BDA9-CD1A-4469-A748-B3533451AED9}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.5546875" customWidth="1"/>
     <col min="2" max="2" width="116.109375" customWidth="1"/>
@@ -970,7 +963,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C2" s="8"/>
     </row>
@@ -979,7 +972,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C3" s="8">
         <v>20</v>
@@ -990,7 +983,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C4" s="9">
         <v>80</v>
@@ -1009,12 +1002,12 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B8" s="11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1030,7 +1023,7 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.88671875" customWidth="1"/>
     <col min="2" max="2" width="66.5546875" customWidth="1"/>
@@ -1043,13 +1036,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>9</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -1057,13 +1050,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="19" t="s">
         <v>20</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -1071,13 +1064,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -1085,13 +1078,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="D4" s="20" t="s">
         <v>27</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -1099,13 +1092,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="D5" s="20" t="s">
         <v>28</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -1113,13 +1106,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -1127,13 +1120,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -1141,13 +1134,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -1155,13 +1148,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="20" t="s">
         <v>37</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="20" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="34.799999999999997" x14ac:dyDescent="0.3">
@@ -1169,13 +1162,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -1183,13 +1176,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="21" t="s">
         <v>42</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>44</v>
       </c>
       <c r="E11" s="12"/>
     </row>
@@ -1272,13 +1265,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA170A17-B9E1-4EAC-B91E-27670B2B139F}">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.5546875" customWidth="1"/>
     <col min="2" max="2" width="101.5546875" customWidth="1"/>
@@ -1286,7 +1279,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="28" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B1" s="28"/>
     </row>
@@ -1295,15 +1288,15 @@
         <v>5</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -1311,7 +1304,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1319,7 +1312,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -1327,12 +1320,12 @@
         <v>3</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="28" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B7" s="28"/>
     </row>
@@ -1341,15 +1334,15 @@
         <v>5</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -1357,7 +1350,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -1365,7 +1358,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1373,12 +1366,12 @@
         <v>3</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="28" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B13" s="28"/>
     </row>
@@ -1387,15 +1380,15 @@
         <v>5</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -1403,7 +1396,7 @@
         <v>2</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -1411,7 +1404,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -1419,12 +1412,12 @@
         <v>3</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="28" t="s">
-        <v>7</v>
+        <v>59</v>
       </c>
       <c r="B19" s="28"/>
     </row>
@@ -1436,7 +1429,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B21" s="23"/>
     </row>
@@ -1450,7 +1443,9 @@
       <c r="A23" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="25"/>
+      <c r="B23" s="25" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="24" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="26" t="s">
@@ -1460,7 +1455,7 @@
     </row>
     <row r="25" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="28" t="s">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="B25" s="28"/>
     </row>
@@ -1472,7 +1467,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B27" s="23"/>
     </row>
@@ -1480,13 +1475,14 @@
       <c r="A28" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="25"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B29" s="25"/>
+      <c r="B29" s="25" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="30" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="26" t="s">
@@ -1494,8 +1490,47 @@
       </c>
       <c r="B30" s="27"/>
     </row>
+    <row r="31" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" s="28"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="23"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33" s="23"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B34" s="25"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B36" s="27"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="A31:B31"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A13:B13"/>

</xml_diff>